<commit_message>
Added myself to roster
</commit_message>
<xml_diff>
--- a/Documents/Team Info/CubeSatTeamRoster.xlsx
+++ b/Documents/Team Info/CubeSatTeamRoster.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\CubeSat\Documents\Team Info\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Charles Denis</t>
   </si>
@@ -495,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,23 +511,23 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="9"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -536,7 +541,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -550,7 +555,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -564,7 +569,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -575,7 +580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -586,7 +591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -597,7 +602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -611,7 +616,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -622,7 +627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -632,8 +637,11 @@
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -647,51 +655,51 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C23" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added myself to subgroup
</commit_message>
<xml_diff>
--- a/Documents/Team Info/CubeSatTeamRoster.xlsx
+++ b/Documents/Team Info/CubeSatTeamRoster.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\CubeSat\Documents\Team Info\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Charles Denis</t>
   </si>
@@ -500,7 +495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -511,14 +506,14 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="4" max="4" width="25.26953125" style="9"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -527,7 +522,7 @@
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -541,7 +536,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -555,7 +550,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -569,7 +564,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -580,7 +575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -591,7 +586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -602,7 +597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -616,7 +611,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -626,8 +621,11 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -641,7 +639,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -655,51 +653,51 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C23" s="2"/>
     </row>
   </sheetData>

</xml_diff>